<commit_message>
steps are now working, needs more tests to only detect steps
</commit_message>
<xml_diff>
--- a/code/steps/steps.xlsx
+++ b/code/steps/steps.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
     <sheet name="Folha4" sheetId="4" r:id="rId4"/>
-    <sheet name="Folha5" sheetId="5" r:id="rId5"/>
+    <sheet name="testar divisao" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -12545,1500 +12545,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Folha5!$A$1:$A$405</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="405"/>
-                <c:pt idx="0">
-                  <c:v>-27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-21</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-38</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-51</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-51</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-50</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-49</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-36</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-38</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-42</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-21</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-38</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-51</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-51</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-49</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-36</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>-42</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-44</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>-42</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>-38</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>-25</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>-28</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>-42</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>-35</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>-19</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>-17</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>-25</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>-34</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>-31</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>-23</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>-33</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>-20</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>-34</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>-33</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>-27</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>-20</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>-20</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>-44</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>-62</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>-53</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>-19</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>-22</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>-28</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>-32</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>-32</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>-27</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>-21</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>-17</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>-25</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>-23</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>-19</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>-24</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>-21</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>-22</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>-24</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>-22</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>-19</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>-25</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>-34</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>-23</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>-17</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>-27</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>-32</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>-24</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>-7</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>-19</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>-20</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>-37</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>-49</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>-53</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>-51</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>-39</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="398">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="399">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="400">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="401">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="402">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="403">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="404">
-                  <c:v>58</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BAB2-4EDC-8320-A746373B1B4D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="890535456"/>
-        <c:axId val="888177040"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="890535456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="888177040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="888177040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="890535456"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -14200,46 +12706,6 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16859,522 +15325,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -17555,47 +15505,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{792D2DA3-8200-43B0-882A-10C7C9318288}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97A36F3-15C8-49FE-A983-DEFA71341677}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30789,2041 +28698,120 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A405"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A405"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>-23</v>
+      </c>
+      <c r="C1">
+        <v>160</v>
+      </c>
+      <c r="E1">
+        <f>SQRT(A1*A1+B1*B1+C1*C1)</f>
+        <v>161.95369708654385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>-22</v>
+      </c>
+      <c r="C2">
+        <v>160</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E7" si="0">SQRT(A2*A2+B2*B2+C2*C2)</f>
+        <v>161.70343224557726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>-24</v>
+      </c>
+      <c r="C3">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>161.98765385053269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>-22</v>
+      </c>
+      <c r="C4">
+        <v>161</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>162.74519962198579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>-23</v>
+      </c>
+      <c r="C5">
+        <v>160</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>161.84251604569178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>-23</v>
+      </c>
+      <c r="C6">
+        <v>161</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>162.88339387426822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>-38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>-49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>-36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>-38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>-42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>-38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>-49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>-36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>-42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>-44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>-42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>-38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>-42</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>-35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>-17</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>-34</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>-31</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>-23</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180">
-        <v>-34</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181">
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244">
-        <v>-44</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245">
-        <v>-62</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246">
-        <v>-53</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254">
-        <v>-22</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255">
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256">
-        <v>-32</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257">
-        <v>-32</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274">
-        <v>-17</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283">
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288">
-        <v>-22</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307">
-        <v>-22</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332">
-        <v>-34</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342">
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343">
-        <v>-17</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368">
-        <v>-32</v>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389">
-        <v>-37</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390">
-        <v>-49</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391">
-        <v>-53</v>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392">
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393">
-        <v>-39</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405">
-        <v>58</v>
+      <c r="C7">
+        <v>159</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>160.90680532531866</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>